<commit_message>
Criação das classes AdicionarLinhas, EmpurrarLinhasParaBaixo e atualização da classe EscritorExcelModelo (merge linhas, estilo e tipo
</commit_message>
<xml_diff>
--- a/Orçamento Alex.xlsx
+++ b/Orçamento Alex.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Orçamento</t>
   </si>
@@ -92,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,12 +180,68 @@
         <v>100.0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>300.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>300.0</v>
+      </c>
+    </row>
     <row r="11">
-      <c r="C11" t="s" s="0">
+      <c r="A11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="n" s="0">
-        <v>850.0</v>
+      <c r="D15" t="n" s="0">
+        <v>1300.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>